<commit_message>
phase 2 & 3
</commit_message>
<xml_diff>
--- a/files/report.xlsx
+++ b/files/report.xlsx
@@ -14,17 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19" count="19">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14" count="14">
   <x:si>
     <x:t>_id</x:t>
   </x:si>
   <x:si>
+    <x:t>date</x:t>
+  </x:si>
+  <x:si>
     <x:t>time</x:t>
   </x:si>
   <x:si>
-    <x:t>date</x:t>
-  </x:si>
-  <x:si>
     <x:t>mandal</x:t>
   </x:si>
   <x:si>
@@ -43,34 +43,19 @@
     <x:t>__v</x:t>
   </x:si>
   <x:si>
-    <x:t>5da1e81322614f2818cc5900</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sat Oct 12 2019 20:19:55 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sat Oct 12 2019 20:19:55 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"dist":"Krishna","mandal":"vij","mroName":"Chiruhas","mroPhone":"7386732234","hasWhatsApp":"false","hasTelegram":"true"}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5da1f4b7c44fb919c0c25b71</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sat Oct 12 2019 20:19:55 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5da1f527c44fb919c0c25b72</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sat Oct 12 2019 20:19:55 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5da1f529c44fb919c0c25b73</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sat Oct 12 2019 20:19:55 GMT+0530 (India Standard Time)</x:t>
+    <x:t>5dd69de6fa189d2ae048845c</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thu Nov 21 2019 00:00:00 GMT+0530 (India Standard Time)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19:45:09</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{"_id":"5dab54277715631de4b15d13","dist":"Srikakulam","mandal":"Veeraghattam","mroPhone":"7995995849","hasTelegram":true,"hasWhatsApp":false,"mroName":"#N/a","__v":0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19:53</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -479,102 +464,15 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="G2" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
       <x:c r="H2" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="I2" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:9">
-      <x:c r="A3" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="I3" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:9">
-      <x:c r="A4" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="I4" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:9">
-      <x:c r="A5" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>